<commit_message>
Name Change In xml Files
</commit_message>
<xml_diff>
--- a/InputData/DataProvider_FrontOffice.xlsx
+++ b/InputData/DataProvider_FrontOffice.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA02211-A970-4C46-8CC4-E01B3E541B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88562B2-DE2A-4064-8378-BBEEDCBC8633}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FO_Registration_Page" sheetId="15" r:id="rId1"/>
-    <sheet name="FO_Billing_Page" sheetId="17" r:id="rId2"/>
-    <sheet name="FO_Appointment_Scheduling" sheetId="18" r:id="rId3"/>
-    <sheet name="FrontOfficeAppointmentSchedul" sheetId="1" r:id="rId4"/>
-    <sheet name="FrontOfficeEquipmentSchedule" sheetId="2" r:id="rId5"/>
-    <sheet name="FrontOfficeDoctorCurrentStatus" sheetId="3" r:id="rId6"/>
-    <sheet name="FrontOfficeSearchSchedule" sheetId="4" r:id="rId7"/>
-    <sheet name="FrontOfficePhysicianOrderbill" sheetId="5" r:id="rId8"/>
-    <sheet name="FrontOfficePatientRegistration" sheetId="7" r:id="rId9"/>
-    <sheet name="FrontOfficeHomeCareAppointment" sheetId="8" r:id="rId10"/>
-    <sheet name="FrontOfficeBlockHomeCareAppo" sheetId="9" r:id="rId11"/>
-    <sheet name="FrontOfficePhyOrderReBilling" sheetId="12" r:id="rId12"/>
-    <sheet name="FrontOfficeUploadDocument" sheetId="13" r:id="rId13"/>
+    <sheet name="FO_Registration_Passport_Page" sheetId="19" r:id="rId2"/>
+    <sheet name="FO_Billing_Page" sheetId="17" r:id="rId3"/>
+    <sheet name="FO_Appointment_Scheduling" sheetId="18" r:id="rId4"/>
+    <sheet name="FrontOfficeAppointmentSchedul" sheetId="1" r:id="rId5"/>
+    <sheet name="FrontOfficeEquipmentSchedule" sheetId="2" r:id="rId6"/>
+    <sheet name="FrontOfficeDoctorCurrentStatus" sheetId="3" r:id="rId7"/>
+    <sheet name="FrontOfficeSearchSchedule" sheetId="4" r:id="rId8"/>
+    <sheet name="FrontOfficePhysicianOrderbill" sheetId="5" r:id="rId9"/>
+    <sheet name="FrontOfficePatientRegistration" sheetId="7" r:id="rId10"/>
+    <sheet name="FrontOfficeHomeCareAppointment" sheetId="8" r:id="rId11"/>
+    <sheet name="FrontOfficeBlockHomeCareAppo" sheetId="9" r:id="rId12"/>
+    <sheet name="FrontOfficePhyOrderReBilling" sheetId="12" r:id="rId13"/>
+    <sheet name="FrontOfficeUploadDocument" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="379">
   <si>
     <t>Facility</t>
   </si>
@@ -882,15 +883,9 @@
     <t>asvg123</t>
   </si>
   <si>
-    <t>Modification</t>
-  </si>
-  <si>
     <t>VIP_Text</t>
   </si>
   <si>
-    <t>Adhar000</t>
-  </si>
-  <si>
     <t xml:space="preserve">ABHA </t>
   </si>
   <si>
@@ -1035,9 +1030,6 @@
     <t>Select_Doctor_name</t>
   </si>
   <si>
-    <t>anannda ji Kumar</t>
-  </si>
-  <si>
     <t>Appoint_First_Name</t>
   </si>
   <si>
@@ -1117,6 +1109,69 @@
   </si>
   <si>
     <t>Under_10_years_DOB</t>
+  </si>
+  <si>
+    <t>ID1234567</t>
+  </si>
+  <si>
+    <t>Remaks Show  In Billing</t>
+  </si>
+  <si>
+    <t>Enter_dig_pin</t>
+  </si>
+  <si>
+    <t>A123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Card Missing </t>
+  </si>
+  <si>
+    <t>Passport_Number</t>
+  </si>
+  <si>
+    <t>Passport_Issued_At</t>
+  </si>
+  <si>
+    <t>Passport_Issue_date</t>
+  </si>
+  <si>
+    <t>Passport_Expiry_date</t>
+  </si>
+  <si>
+    <t>Visa_Vaild_From</t>
+  </si>
+  <si>
+    <t>Visa_Number</t>
+  </si>
+  <si>
+    <t>Visa_valid_to</t>
+  </si>
+  <si>
+    <t>Passport_Remaks</t>
+  </si>
+  <si>
+    <t>PassportNO001</t>
+  </si>
+  <si>
+    <t>NEW DELHI</t>
+  </si>
+  <si>
+    <t>VISANUMBER001</t>
+  </si>
+  <si>
+    <t>Check And Save</t>
+  </si>
+  <si>
+    <t>Satish</t>
+  </si>
+  <si>
+    <t>city_drp</t>
+  </si>
+  <si>
+    <t>New Delhi D345</t>
+  </si>
+  <si>
+    <t>Bobby Lord</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E013439-B5E0-44E3-AE81-9E94621FE47E}">
-  <dimension ref="A1:BJ2"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
-      <selection sqref="A1:BJ2"/>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,43 +1547,44 @@
     <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="30" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="25" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="31" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" customWidth="1"/>
+    <col min="28" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="30" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" customWidth="1"/>
+    <col min="39" max="39" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="31" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -1554,7 +1610,7 @@
         <v>211</v>
       </c>
       <c r="I1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>212</v>
@@ -1607,121 +1663,124 @@
       <c r="Z1" t="s">
         <v>226</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB1" t="s">
         <v>227</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>228</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>229</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>230</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>231</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>232</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>233</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>235</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>236</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>237</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>238</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>239</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>240</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>241</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>242</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>243</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>244</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>246</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>247</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>248</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>249</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>250</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>251</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>252</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>253</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>254</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>255</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>257</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>258</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>259</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>260</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
@@ -1745,7 +1804,7 @@
         <v>43058</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="K2" t="s">
         <v>94</v>
@@ -1766,7 +1825,7 @@
         <v>12345678</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R2">
         <v>9876543210</v>
@@ -1784,124 +1843,127 @@
         <v>271</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="X2" t="s">
         <v>273</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Z2" t="s">
         <v>274</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="AB2" t="s">
         <v>275</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>276</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>277</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>278</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>279</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>280</v>
       </c>
       <c r="AG2" t="s">
         <v>280</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>362</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>359</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>358</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>284</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>291</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>292</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE2" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="AI2" t="s">
-        <v>281</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>282</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>283</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>284</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>285</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>286</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AS2" s="5" t="s">
+      <c r="BF2" t="s">
+        <v>293</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>294</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="AT2" t="s">
-        <v>287</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>288</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>289</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>290</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>291</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>292</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>293</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>294</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>189</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>190</v>
-      </c>
-      <c r="BD2" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="BE2" t="s">
+      <c r="BK2" t="s">
         <v>295</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>296</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>189</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>190</v>
-      </c>
-      <c r="BI2" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -1914,6 +1976,158 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -2062,7 +2276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2132,7 +2346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2181,7 +2395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
@@ -2448,6 +2662,219 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B46374-9208-47E4-93A3-0C8576411B23}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G1" t="s">
+        <v>368</v>
+      </c>
+      <c r="H1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J1" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P1" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>357</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="S1" t="s">
+        <v>213</v>
+      </c>
+      <c r="T1" t="s">
+        <v>217</v>
+      </c>
+      <c r="U1" t="s">
+        <v>221</v>
+      </c>
+      <c r="V1" t="s">
+        <v>376</v>
+      </c>
+      <c r="W1" t="s">
+        <v>222</v>
+      </c>
+      <c r="X1" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" s="3">
+        <v>46344</v>
+      </c>
+      <c r="E2" s="3">
+        <v>46016</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45610</v>
+      </c>
+      <c r="I2" s="3">
+        <v>46140</v>
+      </c>
+      <c r="J2" t="s">
+        <v>374</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
+        <v>375</v>
+      </c>
+      <c r="M2" t="s">
+        <v>263</v>
+      </c>
+      <c r="N2" t="s">
+        <v>203</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3">
+        <v>40499</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>43058</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="S2" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" t="s">
+        <v>377</v>
+      </c>
+      <c r="V2" t="s">
+        <v>272</v>
+      </c>
+      <c r="W2" t="s">
+        <v>271</v>
+      </c>
+      <c r="X2" t="s">
+        <v>280</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373D655A-26ED-4DBB-8B5A-A69FDF4C415A}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -2482,46 +2909,46 @@
         <v>205</v>
       </c>
       <c r="C1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" t="s">
         <v>305</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>307</v>
       </c>
-      <c r="E1" t="s">
-        <v>309</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="G1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L1" t="s">
+        <v>319</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="O1" t="s">
+        <v>323</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="G1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H1" t="s">
-        <v>314</v>
-      </c>
-      <c r="I1" t="s">
-        <v>312</v>
-      </c>
-      <c r="J1" t="s">
-        <v>313</v>
-      </c>
-      <c r="K1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L1" t="s">
-        <v>321</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="O1" t="s">
-        <v>325</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2529,49 +2956,49 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" t="s">
         <v>306</v>
       </c>
-      <c r="D2" t="s">
-        <v>308</v>
-      </c>
       <c r="E2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>328</v>
-      </c>
       <c r="G2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H2" t="s">
         <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L2" t="s">
         <v>320</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
       </c>
       <c r="P2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2580,12 +3007,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3078705D-F9CA-4876-A484-E54C9F60570C}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,55 +3045,55 @@
         <v>205</v>
       </c>
       <c r="C1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E1" t="s">
         <v>331</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>332</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1" t="s">
         <v>334</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>336</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>337</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" t="s">
         <v>338</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>339</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>340</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>341</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>342</v>
-      </c>
-      <c r="N1" t="s">
-        <v>343</v>
-      </c>
-      <c r="O1" t="s">
-        <v>344</v>
-      </c>
-      <c r="P1" t="s">
-        <v>345</v>
       </c>
       <c r="Q1" t="s">
         <v>113</v>
       </c>
       <c r="R1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="S1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2674,58 +3101,58 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>378</v>
       </c>
       <c r="E2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H2">
         <v>8527417</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="L2" t="s">
         <v>129</v>
       </c>
       <c r="M2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
+        <v>351</v>
+      </c>
+      <c r="P2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>352</v>
+      </c>
+      <c r="R2" t="s">
         <v>354</v>
       </c>
-      <c r="P2" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>355</v>
-      </c>
-      <c r="R2" t="s">
-        <v>357</v>
-      </c>
       <c r="S2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -2734,7 +3161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW2"/>
   <sheetViews>
@@ -3095,7 +3522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -3247,7 +3674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3325,7 +3752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3410,7 +3837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3580,156 +4007,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="5"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" t="s">
-        <v>104</v>
-      </c>
-      <c r="P1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Appointment and Fo Billing
</commit_message>
<xml_diff>
--- a/InputData/DataProvider_FrontOffice.xlsx
+++ b/InputData/DataProvider_FrontOffice.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88562B2-DE2A-4064-8378-BBEEDCBC8633}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C3FBF-524D-401C-BD8E-36566E2FA372}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FO_Registration_Page" sheetId="15" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="390">
   <si>
     <t>Facility</t>
   </si>
@@ -964,9 +964,6 @@
     <t>Diagnostics_Test_Name</t>
   </si>
   <si>
-    <t>CBC</t>
-  </si>
-  <si>
     <t>Diagnostics_Test_Speciality_drp</t>
   </si>
   <si>
@@ -979,9 +976,6 @@
     <t>Anaesthesia</t>
   </si>
   <si>
-    <t>Employee151</t>
-  </si>
-  <si>
     <t>Manual_Service_Name_drp</t>
   </si>
   <si>
@@ -1009,15 +1003,9 @@
     <t>Referred_By</t>
   </si>
   <si>
-    <t>ana</t>
-  </si>
-  <si>
     <t>Visit_Room_numver_drp</t>
   </si>
   <si>
-    <t>111</t>
-  </si>
-  <si>
     <t>Facilitator_Name_Drp</t>
   </si>
   <si>
@@ -1171,7 +1159,52 @@
     <t>New Delhi D345</t>
   </si>
   <si>
-    <t>Bobby Lord</t>
+    <t>Rishab Mishra</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Appointment_Booking_Date</t>
+  </si>
+  <si>
+    <t>Billing_Source_Drp</t>
+  </si>
+  <si>
+    <t>Billing_SubSource_Drp</t>
+  </si>
+  <si>
+    <t>enter_remaks</t>
+  </si>
+  <si>
+    <t>Billing Remaks Box</t>
+  </si>
+  <si>
+    <t>Employee231</t>
+  </si>
+  <si>
+    <t>cbc outsource</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>Laxmi Halder</t>
+  </si>
+  <si>
+    <t>Bill_Scheme_Drp</t>
+  </si>
+  <si>
+    <t>Scheme_Authorised_By_drp</t>
+  </si>
+  <si>
+    <t>Auto_Bill_Scheme_Date</t>
+  </si>
+  <si>
+    <t>Dr. Himanshu Sharma</t>
+  </si>
+  <si>
+    <t>222</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E013439-B5E0-44E3-AE81-9E94621FE47E}">
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BF2" sqref="BF2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,7 +1643,7 @@
         <v>211</v>
       </c>
       <c r="I1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>212</v>
@@ -1664,7 +1697,7 @@
         <v>226</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="AB1" t="s">
         <v>227</v>
@@ -1804,7 +1837,7 @@
         <v>43058</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="K2" t="s">
         <v>94</v>
@@ -1855,7 +1888,7 @@
         <v>274</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AB2" t="s">
         <v>275</v>
@@ -1885,19 +1918,19 @@
         <v>281</v>
       </c>
       <c r="AK2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="AL2" t="s">
         <v>282</v>
       </c>
       <c r="AM2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AN2" t="s">
         <v>101</v>
       </c>
       <c r="AO2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AP2" t="s">
         <v>283</v>
@@ -2705,28 +2738,28 @@
         <v>205</v>
       </c>
       <c r="C1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H1" t="s">
         <v>363</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>365</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>366</v>
-      </c>
-      <c r="F1" t="s">
-        <v>364</v>
-      </c>
-      <c r="G1" t="s">
-        <v>368</v>
-      </c>
-      <c r="H1" t="s">
-        <v>367</v>
-      </c>
-      <c r="I1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J1" t="s">
-        <v>370</v>
       </c>
       <c r="K1" t="s">
         <v>206</v>
@@ -2747,7 +2780,7 @@
         <v>211</v>
       </c>
       <c r="Q1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>212</v>
@@ -2762,7 +2795,7 @@
         <v>221</v>
       </c>
       <c r="V1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="W1" t="s">
         <v>222</v>
@@ -2791,7 +2824,7 @@
         <v>296</v>
       </c>
       <c r="C2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D2" s="3">
         <v>46344</v>
@@ -2800,10 +2833,10 @@
         <v>46016</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H2" s="3">
         <v>45610</v>
@@ -2812,13 +2845,13 @@
         <v>46140</v>
       </c>
       <c r="J2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K2" t="s">
         <v>90</v>
       </c>
       <c r="L2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="M2" t="s">
         <v>263</v>
@@ -2836,7 +2869,7 @@
         <v>43058</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="S2" t="s">
         <v>94</v>
@@ -2845,7 +2878,7 @@
         <v>170</v>
       </c>
       <c r="U2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="V2" t="s">
         <v>272</v>
@@ -2876,10 +2909,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373D655A-26ED-4DBB-8B5A-A69FDF4C415A}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,10 +2931,16 @@
     <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -2918,40 +2957,58 @@
         <v>307</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G1" t="s">
         <v>308</v>
       </c>
       <c r="H1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I1" t="s">
+        <v>309</v>
+      </c>
+      <c r="J1" t="s">
         <v>310</v>
       </c>
-      <c r="J1" t="s">
-        <v>311</v>
-      </c>
       <c r="K1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" t="s">
+        <v>317</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="L1" t="s">
-        <v>319</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>317</v>
-      </c>
       <c r="O1" t="s">
+        <v>321</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>327</v>
+      <c r="Q1" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2962,43 +3019,61 @@
         <v>304</v>
       </c>
       <c r="D2" t="s">
-        <v>306</v>
+        <v>383</v>
       </c>
       <c r="E2" t="s">
-        <v>324</v>
+        <v>384</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>326</v>
+        <v>389</v>
       </c>
       <c r="G2" t="s">
-        <v>309</v>
+        <v>382</v>
       </c>
       <c r="H2" t="s">
         <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J2" t="s">
-        <v>314</v>
+        <v>381</v>
       </c>
       <c r="K2" t="s">
+        <v>316</v>
+      </c>
+      <c r="L2" t="s">
         <v>318</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
       </c>
       <c r="P2" t="s">
-        <v>328</v>
+        <v>324</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>290</v>
+      </c>
+      <c r="R2" t="s">
+        <v>291</v>
+      </c>
+      <c r="S2" t="s">
+        <v>380</v>
+      </c>
+      <c r="T2" t="s">
+        <v>293</v>
+      </c>
+      <c r="U2" s="2">
+        <v>45994</v>
+      </c>
+      <c r="V2" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3009,10 +3084,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3078705D-F9CA-4876-A484-E54C9F60570C}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection sqref="A1:S2"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,24 +3095,26 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -3045,58 +3122,61 @@
         <v>205</v>
       </c>
       <c r="C1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" t="s">
         <v>329</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>330</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>332</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>333</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>334</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="N1" t="s">
         <v>335</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>336</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>337</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>338</v>
       </c>
-      <c r="M1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N1" t="s">
-        <v>340</v>
-      </c>
-      <c r="O1" t="s">
-        <v>341</v>
-      </c>
-      <c r="P1" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>113</v>
       </c>
-      <c r="R1" t="s">
-        <v>353</v>
-      </c>
       <c r="S1" t="s">
-        <v>355</v>
+        <v>349</v>
+      </c>
+      <c r="T1" t="s">
+        <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3107,52 +3187,55 @@
         <v>306</v>
       </c>
       <c r="D2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45993</v>
+      </c>
+      <c r="F2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2">
+        <v>8527417</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="K2" t="s">
+        <v>342</v>
+      </c>
+      <c r="L2" t="s">
         <v>343</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" t="s">
         <v>344</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q2" t="s">
         <v>345</v>
       </c>
-      <c r="H2">
-        <v>8527417</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="R2" t="s">
+        <v>348</v>
+      </c>
+      <c r="S2" t="s">
         <v>350</v>
       </c>
-      <c r="J2" t="s">
-        <v>346</v>
-      </c>
-      <c r="K2" t="s">
-        <v>347</v>
-      </c>
-      <c r="L2" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" t="s">
-        <v>348</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>351</v>
-      </c>
-      <c r="P2" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>352</v>
-      </c>
-      <c r="R2" t="s">
-        <v>354</v>
-      </c>
-      <c r="S2" t="s">
-        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Folder Add Nursing Pharmacy lab
</commit_message>
<xml_diff>
--- a/InputData/DataProvider_FrontOffice.xlsx
+++ b/InputData/DataProvider_FrontOffice.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B5DB43-530D-4157-B335-08A84C9F8AAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1035A38C-E4F1-4B7A-A54F-3DC5EB14A667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="59" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="64" activeTab="66" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FO_Registration_Page" sheetId="15" r:id="rId1"/>
@@ -71,6 +71,10 @@
     <sheet name="IP_Pending_Investigation" sheetId="78" r:id="rId61"/>
     <sheet name="IP_Credit_Limit" sheetId="79" r:id="rId62"/>
     <sheet name="IP_General_OrderEntry" sheetId="80" r:id="rId63"/>
+    <sheet name="Nursing_Clearance_Page" sheetId="81" r:id="rId64"/>
+    <sheet name="Pharmacy_Discharge_Notification" sheetId="83" r:id="rId65"/>
+    <sheet name="Lab_Clearance_Page" sheetId="84" r:id="rId66"/>
+    <sheet name="Nursing_Activity_Page" sheetId="85" r:id="rId67"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="984">
   <si>
     <t>SANITY HOSPITAL</t>
   </si>
@@ -3007,6 +3011,33 @@
   </si>
   <si>
     <t>To_Date_Search</t>
+  </si>
+  <si>
+    <t>Nursing_Station_Drp</t>
+  </si>
+  <si>
+    <t>Enter_Date_Expected_Discharge</t>
+  </si>
+  <si>
+    <t>Type_Patient_Drp</t>
+  </si>
+  <si>
+    <t>Billing_Type_Drp</t>
+  </si>
+  <si>
+    <t>Enter_Date_Discharge_Marked</t>
+  </si>
+  <si>
+    <t>Pharmacy_Station_Drp</t>
+  </si>
+  <si>
+    <t>MATERIAL CENTRAL STORE</t>
+  </si>
+  <si>
+    <t>Pharmacy_Status_Drp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st Floor NS </t>
   </si>
 </sst>
 </file>
@@ -7916,8 +7947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F9016A-938F-4400-83E8-235BA46C870F}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10676,8 +10707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D536C2E-2049-4378-975D-D0690C151CB0}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection sqref="A1:O2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10791,6 +10822,279 @@
       </c>
       <c r="O2" t="s">
         <v>933</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F09270-1FEE-4D7E-A2B1-067B6E58EC0B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D1" t="s">
+        <v>976</v>
+      </c>
+      <c r="E1" t="s">
+        <v>977</v>
+      </c>
+      <c r="F1" t="s">
+        <v>952</v>
+      </c>
+      <c r="G1" t="s">
+        <v>978</v>
+      </c>
+      <c r="H1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>800</v>
+      </c>
+      <c r="C2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D2" s="1">
+        <v>46055</v>
+      </c>
+      <c r="E2" t="s">
+        <v>848</v>
+      </c>
+      <c r="F2">
+        <v>29344</v>
+      </c>
+      <c r="G2" t="s">
+        <v>523</v>
+      </c>
+      <c r="H2" s="1">
+        <v>46025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C6946A-E358-4DE2-B43D-AD5F7808634C}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D1" t="s">
+        <v>982</v>
+      </c>
+      <c r="E1" t="s">
+        <v>976</v>
+      </c>
+      <c r="F1" t="s">
+        <v>977</v>
+      </c>
+      <c r="G1" t="s">
+        <v>952</v>
+      </c>
+      <c r="H1" t="s">
+        <v>978</v>
+      </c>
+      <c r="I1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>981</v>
+      </c>
+      <c r="C2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E2" s="1">
+        <v>46054</v>
+      </c>
+      <c r="F2" t="s">
+        <v>848</v>
+      </c>
+      <c r="G2">
+        <v>29344</v>
+      </c>
+      <c r="H2" t="s">
+        <v>910</v>
+      </c>
+      <c r="I2" s="1">
+        <v>46057</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2753D503-B7CA-43F7-BD19-60134A1E726F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D1" t="s">
+        <v>976</v>
+      </c>
+      <c r="E1" t="s">
+        <v>977</v>
+      </c>
+      <c r="F1" t="s">
+        <v>952</v>
+      </c>
+      <c r="G1" t="s">
+        <v>978</v>
+      </c>
+      <c r="H1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>983</v>
+      </c>
+      <c r="C2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D2" s="1">
+        <v>46027</v>
+      </c>
+      <c r="E2" t="s">
+        <v>848</v>
+      </c>
+      <c r="F2">
+        <v>23564</v>
+      </c>
+      <c r="G2" t="s">
+        <v>523</v>
+      </c>
+      <c r="H2" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B73523-0C7D-4155-AC44-E87812CD37B8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>